<commit_message>
ExtraFields added to samples
</commit_message>
<xml_diff>
--- a/DataMan/Records/static/download-template-Price.xlsx
+++ b/DataMan/Records/static/download-template-Price.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M McCown\SCS\DataMan\Records\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6536F1D-DC67-4488-A487-BC3F86FE56E9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC78049-8CAE-434B-A14A-7072B3CED1E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10320" yWindow="1104" windowWidth="12180" windowHeight="10860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataMan Upload Instructions" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="206">
   <si>
     <t>Species</t>
   </si>
@@ -1770,6 +1770,15 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1847,15 +1856,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2201,230 +2201,230 @@
       <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="118" t="s">
+      <c r="A2" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="118"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
-      <c r="H2" s="118"/>
-      <c r="I2" s="118"/>
-      <c r="J2" s="118"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="119" t="s">
+      <c r="A3" s="122" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="119"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
+      <c r="H3" s="122"/>
+      <c r="I3" s="122"/>
+      <c r="J3" s="122"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="121" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
-      <c r="I4" s="118"/>
-      <c r="J4" s="118"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="121"/>
+      <c r="J4" s="121"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="118" t="s">
+      <c r="A5" s="121" t="s">
         <v>104</v>
       </c>
-      <c r="B5" s="118"/>
-      <c r="C5" s="118"/>
-      <c r="D5" s="118"/>
-      <c r="E5" s="118"/>
-      <c r="F5" s="118"/>
-      <c r="G5" s="118"/>
-      <c r="H5" s="118"/>
-      <c r="I5" s="118"/>
-      <c r="J5" s="118"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="118"/>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="118"/>
-      <c r="J6" s="118"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
+      <c r="I6" s="121"/>
+      <c r="J6" s="121"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="121" t="s">
         <v>97</v>
       </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
-      <c r="G7" s="118"/>
-      <c r="H7" s="118"/>
-      <c r="I7" s="118"/>
-      <c r="J7" s="118"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="121"/>
+      <c r="J7" s="121"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="118"/>
-      <c r="B8" s="118"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="118"/>
-      <c r="I8" s="118"/>
-      <c r="J8" s="118"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="121" t="s">
         <v>154</v>
       </c>
-      <c r="B9" s="118"/>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118"/>
-      <c r="E9" s="118"/>
-      <c r="F9" s="118"/>
-      <c r="G9" s="118"/>
-      <c r="H9" s="118"/>
-      <c r="I9" s="118"/>
-      <c r="J9" s="118"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="121"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
+      <c r="J9" s="121"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="118"/>
-      <c r="B10" s="118"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="118"/>
-      <c r="E10" s="118"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="118"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="118"/>
-      <c r="J10" s="118"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="121"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121"/>
+      <c r="G10" s="121"/>
+      <c r="H10" s="121"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="121"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="121" t="s">
         <v>155</v>
       </c>
-      <c r="B11" s="118"/>
-      <c r="C11" s="118"/>
-      <c r="D11" s="118"/>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
-      <c r="J11" s="118"/>
+      <c r="B11" s="121"/>
+      <c r="C11" s="121"/>
+      <c r="D11" s="121"/>
+      <c r="E11" s="121"/>
+      <c r="F11" s="121"/>
+      <c r="G11" s="121"/>
+      <c r="H11" s="121"/>
+      <c r="I11" s="121"/>
+      <c r="J11" s="121"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="118" t="s">
+      <c r="A12" s="121" t="s">
         <v>156</v>
       </c>
-      <c r="B12" s="118"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="118"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="121"/>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="F12" s="121"/>
+      <c r="G12" s="121"/>
+      <c r="H12" s="121"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="121"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="118"/>
-      <c r="B13" s="118"/>
-      <c r="C13" s="118"/>
-      <c r="D13" s="118"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
-      <c r="J13" s="118"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="121"/>
+      <c r="C13" s="121"/>
+      <c r="D13" s="121"/>
+      <c r="E13" s="121"/>
+      <c r="F13" s="121"/>
+      <c r="G13" s="121"/>
+      <c r="H13" s="121"/>
+      <c r="I13" s="121"/>
+      <c r="J13" s="121"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="121" t="s">
         <v>162</v>
       </c>
-      <c r="B14" s="118"/>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="118"/>
+      <c r="B14" s="121"/>
+      <c r="C14" s="121"/>
+      <c r="D14" s="121"/>
+      <c r="E14" s="121"/>
+      <c r="F14" s="121"/>
+      <c r="G14" s="121"/>
+      <c r="H14" s="121"/>
+      <c r="I14" s="121"/>
+      <c r="J14" s="121"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="118"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="121"/>
+      <c r="C15" s="121"/>
+      <c r="D15" s="121"/>
+      <c r="E15" s="121"/>
+      <c r="F15" s="121"/>
+      <c r="G15" s="121"/>
+      <c r="H15" s="121"/>
+      <c r="I15" s="121"/>
+      <c r="J15" s="121"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="118" t="s">
+      <c r="A16" s="121" t="s">
         <v>157</v>
       </c>
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="121"/>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="121"/>
+      <c r="I16" s="121"/>
+      <c r="J16" s="121"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="118" t="s">
+      <c r="A17" s="121" t="s">
         <v>158</v>
       </c>
-      <c r="B17" s="118"/>
-      <c r="C17" s="118"/>
-      <c r="D17" s="118"/>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
+      <c r="B17" s="121"/>
+      <c r="C17" s="121"/>
+      <c r="D17" s="121"/>
+      <c r="E17" s="121"/>
+      <c r="F17" s="121"/>
+      <c r="G17" s="121"/>
+      <c r="H17" s="121"/>
+      <c r="I17" s="121"/>
+      <c r="J17" s="121"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="118"/>
-      <c r="B18" s="118"/>
-      <c r="C18" s="118"/>
-      <c r="D18" s="118"/>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="118"/>
+      <c r="A18" s="121"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="121"/>
+      <c r="D18" s="121"/>
+      <c r="E18" s="121"/>
+      <c r="F18" s="121"/>
+      <c r="G18" s="121"/>
+      <c r="H18" s="121"/>
+      <c r="I18" s="121"/>
+      <c r="J18" s="121"/>
     </row>
     <row r="19" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="43" t="s">
@@ -2449,17 +2449,17 @@
       <c r="A21" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="118" t="s">
+      <c r="B21" s="121" t="s">
         <v>159</v>
       </c>
-      <c r="C21" s="118"/>
-      <c r="D21" s="118"/>
-      <c r="E21" s="118"/>
-      <c r="F21" s="118"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="118"/>
-      <c r="I21" s="118"/>
-      <c r="J21" s="118"/>
+      <c r="C21" s="121"/>
+      <c r="D21" s="121"/>
+      <c r="E21" s="121"/>
+      <c r="F21" s="121"/>
+      <c r="G21" s="121"/>
+      <c r="H21" s="121"/>
+      <c r="I21" s="121"/>
+      <c r="J21" s="121"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -2888,11 +2888,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A17:J17"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="B21:J21"/>
     <mergeCell ref="A14:J14"/>
@@ -2906,6 +2901,11 @@
     <mergeCell ref="A12:J12"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3283,7 +3283,7 @@
   <dimension ref="A1:O1007"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3301,16 +3301,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="127" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="126"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="129"/>
       <c r="I1" s="109" t="s">
         <v>66</v>
       </c>
@@ -3319,104 +3319,104 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="131" t="s">
+      <c r="A2" s="134" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="133"/>
-      <c r="D2" s="133"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="133"/>
-      <c r="G2" s="133"/>
-      <c r="H2" s="134"/>
+      <c r="B2" s="135"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="136"/>
+      <c r="E2" s="136"/>
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="137"/>
       <c r="I2" s="110" t="s">
         <v>0</v>
       </c>
       <c r="J2" s="58"/>
     </row>
     <row r="3" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A3" s="137" t="s">
+      <c r="A3" s="140" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="138"/>
-      <c r="C3" s="135" t="s">
+      <c r="B3" s="141"/>
+      <c r="C3" s="138" t="s">
         <v>194</v>
       </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="135"/>
-      <c r="G3" s="135"/>
-      <c r="H3" s="136"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="139"/>
       <c r="I3" s="111" t="s">
         <v>82</v>
       </c>
       <c r="J3" s="61"/>
     </row>
     <row r="4" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A4" s="137" t="s">
+      <c r="A4" s="140" t="s">
         <v>179</v>
       </c>
-      <c r="B4" s="138"/>
-      <c r="C4" s="145"/>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
-      <c r="F4" s="145"/>
-      <c r="G4" s="144"/>
-      <c r="H4" s="146"/>
+      <c r="B4" s="141"/>
+      <c r="C4" s="119"/>
+      <c r="D4" s="118"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="119"/>
+      <c r="G4" s="118"/>
+      <c r="H4" s="120"/>
       <c r="I4" s="112" t="s">
         <v>83</v>
       </c>
       <c r="J4" s="59"/>
     </row>
     <row r="5" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="127" t="s">
+      <c r="A5" s="130" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="129"/>
+      <c r="B5" s="131"/>
+      <c r="C5" s="131"/>
+      <c r="D5" s="131"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="131"/>
+      <c r="G5" s="131"/>
+      <c r="H5" s="132"/>
       <c r="I5" s="113" t="s">
         <v>1</v>
       </c>
       <c r="J5" s="62"/>
     </row>
     <row r="6" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="130"/>
-      <c r="B6" s="128"/>
-      <c r="C6" s="128"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="129"/>
+      <c r="A6" s="133"/>
+      <c r="B6" s="131"/>
+      <c r="C6" s="131"/>
+      <c r="D6" s="131"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="131"/>
+      <c r="G6" s="131"/>
+      <c r="H6" s="132"/>
       <c r="I6" s="114" t="s">
         <v>22</v>
       </c>
       <c r="J6" s="60"/>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="130"/>
-      <c r="B7" s="128"/>
-      <c r="C7" s="128"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="129"/>
+      <c r="A7" s="133"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="131"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="131"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="132"/>
     </row>
     <row r="8" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A8" s="130"/>
-      <c r="B8" s="128"/>
-      <c r="C8" s="128"/>
-      <c r="D8" s="128"/>
-      <c r="E8" s="128"/>
-      <c r="F8" s="128"/>
-      <c r="G8" s="128"/>
-      <c r="H8" s="129"/>
+      <c r="A8" s="133"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="131"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="131"/>
+      <c r="G8" s="131"/>
+      <c r="H8" s="132"/>
       <c r="I8" s="115" t="s">
         <v>2</v>
       </c>
@@ -3425,14 +3425,14 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A9" s="130"/>
-      <c r="B9" s="128"/>
-      <c r="C9" s="128"/>
-      <c r="D9" s="128"/>
-      <c r="E9" s="128"/>
-      <c r="F9" s="128"/>
-      <c r="G9" s="128"/>
-      <c r="H9" s="129"/>
+      <c r="A9" s="133"/>
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="132"/>
       <c r="I9" s="116" t="s">
         <v>5</v>
       </c>
@@ -3441,16 +3441,16 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="122" t="s">
+      <c r="A10" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="B10" s="123"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="120"/>
-      <c r="G10" s="120"/>
-      <c r="H10" s="121"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="123"/>
+      <c r="D10" s="123"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="124"/>
       <c r="I10" s="117" t="s">
         <v>3</v>
       </c>
@@ -3530,9 +3530,7 @@
       <c r="M15" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="N15" s="7" t="s">
-        <v>84</v>
-      </c>
+      <c r="N15" s="7"/>
       <c r="O15" s="7"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -11124,7 +11122,7 @@
         <v>183</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" ref="C3:C14" si="0">CONCATENATE($L$9,A4)</f>
+        <f t="shared" ref="C4:C14" si="0">CONCATENATE($L$9,A4)</f>
         <v>C:\Xcalibur\methods\30_min_simple</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -11316,64 +11314,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="142" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="139"/>
-      <c r="G1" s="139"/>
-      <c r="H1" s="140"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="142"/>
+      <c r="E1" s="142"/>
+      <c r="F1" s="142"/>
+      <c r="G1" s="142"/>
+      <c r="H1" s="143"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="141" t="s">
+      <c r="A2" s="144" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="142"/>
-      <c r="C2" s="142"/>
-      <c r="D2" s="142"/>
-      <c r="E2" s="142"/>
-      <c r="F2" s="142"/>
-      <c r="G2" s="142"/>
-      <c r="H2" s="142"/>
+      <c r="B2" s="145"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="145"/>
+      <c r="E2" s="145"/>
+      <c r="F2" s="145"/>
+      <c r="G2" s="145"/>
+      <c r="H2" s="145"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="121" t="s">
         <v>147</v>
       </c>
-      <c r="B4" s="118"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
-      <c r="G4" s="118"/>
-      <c r="H4" s="118"/>
+      <c r="B4" s="121"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="121"/>
+      <c r="F4" s="121"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="143" t="s">
+      <c r="A5" s="146" t="s">
         <v>168</v>
       </c>
-      <c r="B5" s="143"/>
-      <c r="C5" s="143"/>
-      <c r="D5" s="143"/>
-      <c r="E5" s="143"/>
-      <c r="F5" s="143"/>
-      <c r="G5" s="143"/>
-      <c r="H5" s="143"/>
+      <c r="B5" s="146"/>
+      <c r="C5" s="146"/>
+      <c r="D5" s="146"/>
+      <c r="E5" s="146"/>
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="146"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="118" t="s">
+      <c r="A6" s="121" t="s">
         <v>163</v>
       </c>
-      <c r="B6" s="118"/>
-      <c r="C6" s="118"/>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
+      <c r="B6" s="121"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
+      <c r="F6" s="121"/>
+      <c r="G6" s="121"/>
+      <c r="H6" s="121"/>
     </row>
     <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">

</xml_diff>